<commit_message>
ajout d'une colonne #piece cegep
</commit_message>
<xml_diff>
--- a/TEP_243-Altium_RLC_Librairie.xlsx
+++ b/TEP_243-Altium_RLC_Librairie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lecegeplimoilou-my.sharepoint.com/personal/kevin_cotton_cegeplimoilou_ca/Documents/_Cours-TGE/Altium/Librairies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="361" documentId="13_ncr:1_{550D3E46-E4B6-4165-A45B-7D583CCE157E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6620CB5E-AD73-4F34-8A01-74B1C95A1C3F}"/>
+  <xr:revisionPtr revIDLastSave="368" documentId="13_ncr:1_{550D3E46-E4B6-4165-A45B-7D583CCE157E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A433130E-BE41-44AE-8C7D-55C06E0D2DAE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cap" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="Ind" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cap!$A$1:$R$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Ind!$A$1:$Q$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Res!$A$1:$Q$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cap!$A$1:$S$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Ind!$A$1:$R$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Res!$A$1:$R$15</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="141">
   <si>
     <t>Comment</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t>CAP007</t>
+  </si>
+  <si>
+    <t>CEGEP</t>
   </si>
 </sst>
 </file>
@@ -795,345 +798,348 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" customWidth="1"/>
-    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" customWidth="1"/>
-    <col min="16" max="16" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" customWidth="1"/>
+    <col min="17" max="17" width="19.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>90</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>130</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>0.1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>27</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>36</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>26</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>53</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>0.1</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>17</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>27</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>25</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>37</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>82</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>90</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>132</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>0.1</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>83</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>16</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>17</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>27</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>25</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>97</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>26</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>53</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>85</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>90</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>91</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>0.1</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>84</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>16</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>17</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>27</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>25</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>97</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>26</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>53</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>87</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>86</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>94</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>84</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>96</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>17</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>27</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>25</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>98</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>89</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>88</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>136</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>135</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>95</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>0.05</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>15</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>137</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>17</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>27</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>25</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>36</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>26</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>53</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>139</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:S1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1141,616 +1147,619 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0837104-CD0C-4055-94B3-0A98F94F86E8}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.77734375" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" customWidth="1"/>
-    <col min="15" max="15" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.77734375" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" customWidth="1"/>
+    <col min="13" max="13" width="15.77734375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" customWidth="1"/>
+    <col min="16" max="16" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>70</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>0.01</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>32</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>69</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>0.01</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>32</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>68</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>102</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>101</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>0.01</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>43</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>15</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>17</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>32</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>26</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>99</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>71</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>0.01</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>43</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>15</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>32</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>67</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>78</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>77</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>74</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>15</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>17</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>32</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>26</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>53</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>59</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>72</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>78</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>79</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>0.01</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>43</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>15</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>17</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>32</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>26</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>53</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>60</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>80</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>0.01</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>43</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>15</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>17</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>32</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>26</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>61</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>104</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>78</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>106</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>108</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>0.01</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>43</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>15</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>17</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>32</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>26</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>115</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>100</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>62</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>105</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>102</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>107</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>109</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>0.01</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>43</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>15</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>17</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>32</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>26</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>99</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>63</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>118</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>81</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>124</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>121</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>0.01</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>43</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>15</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>17</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>32</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>26</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>53</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>64</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>119</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>81</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>125</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>122</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>0.01</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>43</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>15</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>17</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>32</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="M12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>26</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>53</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>65</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>120</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>81</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>126</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>123</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>0.01</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>43</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>15</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>17</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>32</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>25</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="M13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>26</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>53</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q15" xr:uid="{C0837104-CD0C-4055-94B3-0A98F94F86E8}"/>
+  <autoFilter ref="A1:R15" xr:uid="{C0837104-CD0C-4055-94B3-0A98F94F86E8}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1758,7 +1767,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A0C756-8EF7-43C5-A896-F15EFC0CC7A5}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1766,138 +1775,141 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
-    <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" customWidth="1"/>
+    <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>48</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>0.2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>56</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>55</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>33</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>49</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>26</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>53</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>34</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>25</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q1" xr:uid="{07A0C756-8EF7-43C5-A896-F15EFC0CC7A5}"/>
+  <autoFilter ref="A1:R1" xr:uid="{07A0C756-8EF7-43C5-A896-F15EFC0CC7A5}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>